<commit_message>
feat: matriz SoD now loads from database.xlsx
</commit_message>
<xml_diff>
--- a/model/backup.xlsx
+++ b/model/backup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>descricao C</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Mm</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>111.222.333-44</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -519,38 +519,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -706,18 +706,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>

<commit_message>
feat: started attempt on user add
</commit_message>
<xml_diff>
--- a/model/backup.xlsx
+++ b/model/backup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">111.222.333-44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">555.666.777-88</t>
   </si>
 </sst>
 </file>
@@ -158,8 +161,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,37 +193,37 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -242,41 +249,41 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -298,170 +305,170 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>0</v>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -481,37 +488,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: changed codigo for sistema in perfil
</commit_message>
<xml_diff>
--- a/model/backup.xlsx
+++ b/model/backup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>codigo</t>
   </si>
@@ -86,54 +86,6 @@
     <t>descricao A</t>
   </si>
   <si>
-    <t>Dd</t>
-  </si>
-  <si>
-    <t>Ds</t>
-  </si>
-  <si>
-    <t>Da</t>
-  </si>
-  <si>
-    <t>Rd</t>
-  </si>
-  <si>
-    <t>Rg</t>
-  </si>
-  <si>
-    <t>Rs</t>
-  </si>
-  <si>
-    <t>Ra</t>
-  </si>
-  <si>
-    <t>Fd</t>
-  </si>
-  <si>
-    <t>Fg</t>
-  </si>
-  <si>
-    <t>Fs</t>
-  </si>
-  <si>
-    <t>Fa</t>
-  </si>
-  <si>
-    <t>Ed</t>
-  </si>
-  <si>
-    <t>Eg</t>
-  </si>
-  <si>
-    <t>Es</t>
-  </si>
-  <si>
-    <t>Ea</t>
-  </si>
-  <si>
-    <t>Dg</t>
-  </si>
-  <si>
     <t>222.333.444-55</t>
   </si>
   <si>
@@ -141,6 +93,54 @@
   </si>
   <si>
     <t>444.555.666-77</t>
+  </si>
+  <si>
+    <t>diretoria - diretor</t>
+  </si>
+  <si>
+    <t>diretoria - gerente</t>
+  </si>
+  <si>
+    <t>diretoria - assessor</t>
+  </si>
+  <si>
+    <t>recursos humanos - diretor</t>
+  </si>
+  <si>
+    <t>recursos humanos - gerente</t>
+  </si>
+  <si>
+    <t>recursos humanos - assessor</t>
+  </si>
+  <si>
+    <t>diretoria - secretaria</t>
+  </si>
+  <si>
+    <t>recursos humanos - secretaria</t>
+  </si>
+  <si>
+    <t>financeiro - diretor</t>
+  </si>
+  <si>
+    <t>financeiro - gerente</t>
+  </si>
+  <si>
+    <t>financeiro - secretaria</t>
+  </si>
+  <si>
+    <t>estoque - diretor</t>
+  </si>
+  <si>
+    <t>estoque - gerente</t>
+  </si>
+  <si>
+    <t>estoque - secretaria</t>
+  </si>
+  <si>
+    <t>estoque - assessor</t>
+  </si>
+  <si>
+    <t>financeiro - assessor</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -557,8 +557,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
@@ -568,8 +568,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
@@ -579,8 +579,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -590,8 +590,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -611,12 +611,13 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="6.7109375" style="3" customWidth="1"/>
+    <col min="1" max="17" width="30.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -624,57 +625,57 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -727,7 +728,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -780,7 +781,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -833,7 +834,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -886,7 +887,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -939,7 +940,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -992,7 +993,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1045,7 +1046,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1098,7 +1099,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -1151,7 +1152,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -1204,7 +1205,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -1257,7 +1258,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
@@ -1310,7 +1311,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3">
         <v>0</v>
@@ -1363,7 +1364,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -1416,7 +1417,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -1469,7 +1470,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -1522,7 +1523,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1565,7 +1566,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1576,7 +1577,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -1587,7 +1588,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
feat: new matriz sod conflict implementation
</commit_message>
<xml_diff>
--- a/model/backup.xlsx
+++ b/model/backup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>codigo</t>
   </si>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +157,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -183,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -192,6 +200,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -477,7 +488,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -535,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1529,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,52 +1564,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: combination saving ongoing
</commit_message>
<xml_diff>
--- a/model/backup.xlsx
+++ b/model/backup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sistemas" sheetId="1" r:id="rId1"/>
@@ -621,14 +621,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="30.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
+    <col min="2" max="17" width="6.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1542,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>